<commit_message>
add some books for buy list
</commit_message>
<xml_diff>
--- a/work/购书.xlsx
+++ b/work/购书.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="198">
   <si>
     <t>书名</t>
   </si>
@@ -718,6 +718,119 @@
   <si>
     <t>黑客与画家</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python基础教程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">斋藤康毅著  陆宇杰译
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python网络编程（第3版）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[美]Brandon Rhodes , [美]John Goerzen (作者) 诸豪文 (译者)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python Cookbook 第三版中文版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">大卫·比斯利 (David Beazley) (作者), 布莱恩·K.琼斯 (Brian K.Jones) (作者), 陈舸 (译者)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人民邮电出版社</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python核心编程（第3版）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[美] Wesley Chun 著，孙波翔，李斌，李晗 译</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深度学习入门：基于Python的理论与实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Http权威指南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人民邮电出版社</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>David Gourley / Brian Totty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用Python进行数据分析（原书第2版）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[美] 韦斯·麦金尼（Wes McKinney）
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">机械工业出版社 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器学习实战</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[美] Peter Harrington</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人民邮电出版社</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络科学引论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mark E. J. Newman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子工业出版社</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据挖掘：实用机器学习工具与技术(原书第3版)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lan H.Witten</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械工业出版社</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++并发编程实战</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[美] Anthony Williams（威廉姆斯） 著，周全，梁娟娟，宋真真，许敏 译</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -745,6 +858,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="DengXian"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -769,7 +883,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -792,13 +906,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -822,6 +947,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1118,15 +1252,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="31.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="44.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.375" style="1" customWidth="1"/>
   </cols>
@@ -1213,7 +1347,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="27">
+    <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
@@ -1345,37 +1479,43 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" ht="27">
       <c r="A21" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="4" t="s">
+      <c r="C22" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-    </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
@@ -1422,82 +1562,82 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="3" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" ht="27">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="27">
+      <c r="A36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="40.5">
-      <c r="A33" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="40.5">
-      <c r="A35" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>17</v>
@@ -1505,83 +1645,182 @@
     </row>
     <row r="37" spans="1:3" ht="27">
       <c r="A37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="40.5">
+      <c r="A39" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="27">
+      <c r="A40" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="54">
+      <c r="A41" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="27">
+      <c r="A42" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="40.5">
+      <c r="A43" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="27">
+      <c r="A44" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="27">
+      <c r="A46" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A38" s="4" t="s">
+    <row r="47" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A47" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="4" t="s">
+    <row r="48" spans="1:3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="3" t="s">
+    <row r="50" spans="1:3">
+      <c r="A50" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="3" t="s">
+      <c r="C50" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="4" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="4" t="s">
+      <c r="C52" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>